<commit_message>
plot 2 graphs on the same dataset
</commit_message>
<xml_diff>
--- a/fastai-excel/Daniel - ReLU.xlsx
+++ b/fastai-excel/Daniel - ReLU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarad\Documents\PMLG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Natsume/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56B1B076-C88B-4014-A2D3-444FA7FA8C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1593B9-F7C6-3749-8999-EF5DE677486C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED7D475E-B212-44E6-B707-CFE7BDCD2AAF}"/>
+    <workbookView xWindow="-120" yWindow="460" windowWidth="29040" windowHeight="15540" xr2:uid="{ED7D475E-B212-44E6-B707-CFE7BDCD2AAF}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,20 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">data!$B$5</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">data!$B$6:$B$26</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">data!$G$5</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">data!$G$6:$G$26</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">data!$H$5</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">data!$H$6:$H$26</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">data!$C$5</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">data!$C$6:$C$26</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">data!$D$5</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">data!$D$6:$D$26</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">data!$E$5</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">data!$E$6:$E$26</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">data!$F$5</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">data!$F$6:$F$26</definedName>
     <definedName name="const_2">#REF!</definedName>
     <definedName name="const2">'[1]basic SGD 2 neuron'!$D$1</definedName>
     <definedName name="inter_b">#REF!</definedName>
@@ -340,7 +354,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -934,7 +948,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="603271024"/>
@@ -993,7 +1007,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="603270608"/>
@@ -1035,7 +1049,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1072,7 +1086,1836 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y=a*x + b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$B$6:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$C$6:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-130</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>270</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3877-6E43-97AF-C5C7D209C60D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y = (a*x + b)*c + d</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$B$6:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$E$6:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-380</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-320</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-260</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-140</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>820</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3877-6E43-97AF-C5C7D209C60D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$H$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y = Z*c + d</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$B$6:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$H$6:$H$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>820</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3877-6E43-97AF-C5C7D209C60D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="269270415"/>
+        <c:axId val="269358687"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>data!$D$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>data!$B$6:$B$26</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="21"/>
+                      <c:pt idx="0">
+                        <c:v>-80</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-70</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-60</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-50</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-40</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-30</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-20</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-10</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>80</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>110</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>120</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>data!$D$6:$D$26</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="21"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-3877-6E43-97AF-C5C7D209C60D}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>data!$F$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>data!$B$6:$B$26</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="21"/>
+                      <c:pt idx="0">
+                        <c:v>-80</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-70</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-60</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-50</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-40</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-30</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-20</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-10</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>80</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>110</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>120</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>data!$F$6:$F$26</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="21"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-3877-6E43-97AF-C5C7D209C60D}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="269270415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="269358687"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="269358687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="269270415"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.0634169168678128E-2"/>
+          <c:y val="0.13550362903125612"/>
+          <c:w val="0.86988888888888893"/>
+          <c:h val="0.67150335374744818"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y=a*x + b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$B$6:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$C$6:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-130</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>270</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E773-3B46-B943-2712DD0DEA2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y = (a*x + b)*c + d</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$B$6:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$E$6:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-380</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-320</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-260</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-140</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>820</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E773-3B46-B943-2712DD0DEA2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$H$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y = Z*c + d</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$B$6:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$H$6:$H$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>820</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E773-3B46-B943-2712DD0DEA2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="269178463"/>
+        <c:axId val="269180111"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="269178463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="269180111"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="269180111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2500"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="269178463"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1123,7 +2966,1119 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1679,6 +4634,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>592667</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>53622</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>423333</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50533C53-FB97-CEDF-0FCB-2997E7321D73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>56444</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>166510</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>437445</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>42334</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9FD2ABB-E67B-0E55-E6EE-CB5FD7946B04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1705,306 +4732,6 @@
         <row r="5">
           <cell r="C5" t="str">
             <v>y=a*x + b</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>y = (a*x + b)*c + d</v>
-          </cell>
-          <cell r="H5" t="str">
-            <v>y = Z*c + d</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>-80</v>
-          </cell>
-          <cell r="C6">
-            <v>-130</v>
-          </cell>
-          <cell r="E6">
-            <v>-380</v>
-          </cell>
-          <cell r="H6">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>-70</v>
-          </cell>
-          <cell r="C7">
-            <v>-110</v>
-          </cell>
-          <cell r="E7">
-            <v>-320</v>
-          </cell>
-          <cell r="H7">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>-60</v>
-          </cell>
-          <cell r="C8">
-            <v>-90</v>
-          </cell>
-          <cell r="E8">
-            <v>-260</v>
-          </cell>
-          <cell r="H8">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>-50</v>
-          </cell>
-          <cell r="C9">
-            <v>-70</v>
-          </cell>
-          <cell r="E9">
-            <v>-200</v>
-          </cell>
-          <cell r="H9">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>-40</v>
-          </cell>
-          <cell r="C10">
-            <v>-50</v>
-          </cell>
-          <cell r="E10">
-            <v>-140</v>
-          </cell>
-          <cell r="H10">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>-30</v>
-          </cell>
-          <cell r="C11">
-            <v>-30</v>
-          </cell>
-          <cell r="E11">
-            <v>-80</v>
-          </cell>
-          <cell r="H11">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>-20</v>
-          </cell>
-          <cell r="C12">
-            <v>-10</v>
-          </cell>
-          <cell r="E12">
-            <v>-20</v>
-          </cell>
-          <cell r="H12">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>-10</v>
-          </cell>
-          <cell r="C13">
-            <v>10</v>
-          </cell>
-          <cell r="E13">
-            <v>40</v>
-          </cell>
-          <cell r="H13">
-            <v>40</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>0</v>
-          </cell>
-          <cell r="C14">
-            <v>30</v>
-          </cell>
-          <cell r="E14">
-            <v>100</v>
-          </cell>
-          <cell r="H14">
-            <v>100</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>10</v>
-          </cell>
-          <cell r="C15">
-            <v>50</v>
-          </cell>
-          <cell r="E15">
-            <v>160</v>
-          </cell>
-          <cell r="H15">
-            <v>160</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>20</v>
-          </cell>
-          <cell r="C16">
-            <v>70</v>
-          </cell>
-          <cell r="E16">
-            <v>220</v>
-          </cell>
-          <cell r="H16">
-            <v>220</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>30</v>
-          </cell>
-          <cell r="C17">
-            <v>90</v>
-          </cell>
-          <cell r="E17">
-            <v>280</v>
-          </cell>
-          <cell r="H17">
-            <v>280</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>40</v>
-          </cell>
-          <cell r="C18">
-            <v>110</v>
-          </cell>
-          <cell r="E18">
-            <v>340</v>
-          </cell>
-          <cell r="H18">
-            <v>340</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>50</v>
-          </cell>
-          <cell r="C19">
-            <v>130</v>
-          </cell>
-          <cell r="E19">
-            <v>400</v>
-          </cell>
-          <cell r="H19">
-            <v>400</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>60</v>
-          </cell>
-          <cell r="C20">
-            <v>150</v>
-          </cell>
-          <cell r="E20">
-            <v>460</v>
-          </cell>
-          <cell r="H20">
-            <v>460</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>70</v>
-          </cell>
-          <cell r="C21">
-            <v>170</v>
-          </cell>
-          <cell r="E21">
-            <v>520</v>
-          </cell>
-          <cell r="H21">
-            <v>520</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>80</v>
-          </cell>
-          <cell r="C22">
-            <v>190</v>
-          </cell>
-          <cell r="E22">
-            <v>580</v>
-          </cell>
-          <cell r="H22">
-            <v>580</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>90</v>
-          </cell>
-          <cell r="C23">
-            <v>210</v>
-          </cell>
-          <cell r="E23">
-            <v>640</v>
-          </cell>
-          <cell r="H23">
-            <v>640</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>100</v>
-          </cell>
-          <cell r="C24">
-            <v>230</v>
-          </cell>
-          <cell r="E24">
-            <v>700</v>
-          </cell>
-          <cell r="H24">
-            <v>700</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>110</v>
-          </cell>
-          <cell r="C25">
-            <v>250</v>
-          </cell>
-          <cell r="E25">
-            <v>760</v>
-          </cell>
-          <cell r="H25">
-            <v>760</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>120</v>
-          </cell>
-          <cell r="C26">
-            <v>270</v>
-          </cell>
-          <cell r="E26">
-            <v>820</v>
-          </cell>
-          <cell r="H26">
-            <v>820</v>
           </cell>
         </row>
       </sheetData>
@@ -2334,23 +5061,23 @@
   <sheetPr codeName="data"/>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2367,7 +5094,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2384,7 +5111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -2401,7 +5128,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>-80</v>
       </c>
@@ -2422,7 +5149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>-70</v>
       </c>
@@ -2443,7 +5170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>-60</v>
       </c>
@@ -2464,7 +5191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>-50</v>
       </c>
@@ -2485,7 +5212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>-40</v>
       </c>
@@ -2506,7 +5233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>-30</v>
       </c>
@@ -2527,7 +5254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>-20</v>
       </c>
@@ -2548,7 +5275,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>-10</v>
       </c>
@@ -2569,7 +5296,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>0</v>
       </c>
@@ -2590,7 +5317,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>10</v>
       </c>
@@ -2611,7 +5338,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>20</v>
       </c>
@@ -2632,7 +5359,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>30</v>
       </c>
@@ -2653,7 +5380,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>40</v>
       </c>
@@ -2674,7 +5401,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>50</v>
       </c>
@@ -2695,7 +5422,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>60</v>
       </c>
@@ -2716,7 +5443,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>70</v>
       </c>
@@ -2737,7 +5464,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>80</v>
       </c>
@@ -2758,7 +5485,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>90</v>
       </c>
@@ -2779,7 +5506,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>100</v>
       </c>
@@ -2800,7 +5527,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>110</v>
       </c>
@@ -2821,7 +5548,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>120</v>
       </c>

</xml_diff>